<commit_message>
Not happy with the EDA, but time to go to sleep
</commit_message>
<xml_diff>
--- a/CH-162 Extract from Text.xlsx
+++ b/CH-162 Extract from Text.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E78ED0-548C-4F4F-BCF0-63F56C55317F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65BDD70-8063-44D1-950C-AACDF3408678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="4" r:id="rId3"/>
+    <sheet name="EDA" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EDA!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -411,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -453,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1682,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DF98BB-10DA-4A65-A2AD-CB24A5B1C420}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -2001,4 +2006,335 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA657A5-5A61-4721-8CFB-2803EF2001BD}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="7" style="5" customWidth="1"/>
+    <col min="6" max="9" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="L1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="12">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="9"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="9"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="18" t="str" cm="1">
+        <f t="array" ref="B12:D12">_xlfn.REGEXEXTRACT(C3,"\{[^}]*\}",1)</f>
+        <v>{1,2,3}</v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <v>{2,3,4}</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <v>{1,2}</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B13" s="18" t="str" cm="1">
+        <f t="array" ref="B13">_xlfn.REGEXEXTRACT(C4,"\{[^}]*\}",1)</f>
+        <v>{1,2,{3,4}</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B14" s="18" t="str" cm="1">
+        <f t="array" ref="B14:C14">_xlfn.REGEXEXTRACT(C5,"\{[^}]*\}",1)</f>
+        <v>{{1,2}</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <v>{3,4}</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="18" t="str" cm="1">
+        <f t="array" ref="B15">_xlfn.REGEXEXTRACT(C6,"\{[^}]*\}",1)</f>
+        <v>{1,2,3}</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="18" t="str" cm="1">
+        <f t="array" ref="B16:C16">_xlfn.REGEXEXTRACT(C7,"\{[^}]*\}",1)</f>
+        <v>{1,{1,{1}</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <v>{1}</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A17" s="1"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A18" s="1"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="4" t="str" cm="1">
+        <f t="array" ref="B19:D19">"{"&amp;_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("-",TRUE,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(C3,"\{{1,2}|\,{{1}|\},{1}|\}","-"),{"-"})),"-")&amp;"}"</f>
+        <v>{1,2,3}</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <v>{2,3,4}</v>
+      </c>
+      <c r="D19" s="10" t="str">
+        <v>{1,2}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4" t="str" cm="1">
+        <f t="array" ref="B20:C20">"{"&amp;_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("-",TRUE,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(C4,"\{{1,2}|\,{{1}|\},{1}|\}","-"),{"-"})),"-")&amp;"}"</f>
+        <v>{1,2}</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <v>{3,4}</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4" t="str" cm="1">
+        <f t="array" ref="B21:C21">"{"&amp;_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("-",TRUE,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(C5,"\{{1,2}|\,{{1}|\},{1}|\}","-"),{"-"})),"-")&amp;"}"</f>
+        <v>{1,2}</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <v>{3,4}</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4" t="str" cm="1">
+        <f t="array" ref="B22">"{"&amp;_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("-",TRUE,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(C6,"\{{1,2}|\,{{1}|\},{1}|\}","-"),{"-"})),"-")&amp;"}"</f>
+        <v>{1,2,3}</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B23" s="4" t="str" cm="1">
+        <f t="array" ref="B23:E23">"{"&amp;_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("-",TRUE,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(C7,"\{{1,2}|\,{{1}|\},{1}|\}","-"),{"-"})),"-")&amp;"}"</f>
+        <v>{1}</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <v>{1}</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v>{1}</v>
+      </c>
+      <c r="E23" s="5" t="str">
+        <v>{1}</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>